<commit_message>
Updated the balance sheet.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
   <si>
     <t>M9</t>
   </si>
@@ -245,15 +245,6 @@
     <t>Move speed</t>
   </si>
   <si>
-    <t>120/70%</t>
-  </si>
-  <si>
-    <t>100/50%</t>
-  </si>
-  <si>
-    <t>80/30%</t>
-  </si>
-  <si>
     <t>60/20%</t>
   </si>
   <si>
@@ -302,10 +293,19 @@
     <t>Plus/minus signs are always relative only within a category</t>
   </si>
   <si>
-    <t>Additional damage multipliers are applied for LMGs (cca. X1.25) and sniper rifles (2x)</t>
-  </si>
-  <si>
-    <t>Last updated 15.3. (r260)</t>
+    <t>150/120%</t>
+  </si>
+  <si>
+    <t>125/110%</t>
+  </si>
+  <si>
+    <t>100/70%</t>
+  </si>
+  <si>
+    <t>Last updated 16.3. (r268)</t>
+  </si>
+  <si>
+    <t>Additional damage multiplieris applied for sniper rifles (2x)</t>
   </si>
 </sst>
 </file>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +744,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="8" max="8" width="6.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.85546875" customWidth="1"/>
@@ -754,7 +755,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -766,7 +767,7 @@
       <c r="I1" s="29"/>
       <c r="J1" s="29"/>
       <c r="K1" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L1" s="33"/>
       <c r="M1" s="33"/>
@@ -774,7 +775,7 @@
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -811,7 +812,7 @@
         <v>58</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>59</v>
@@ -829,7 +830,7 @@
         <v>62</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -843,7 +844,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E4" s="10">
         <v>8</v>
@@ -883,7 +884,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E5" s="5">
         <v>11</v>
@@ -923,7 +924,7 @@
         <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E6" s="5">
         <v>17</v>
@@ -963,7 +964,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E7" s="5">
         <v>26</v>
@@ -975,7 +976,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I7" s="5">
         <v>15</v>
@@ -1003,7 +1004,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E8" s="5">
         <v>11</v>
@@ -1043,7 +1044,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E9" s="5">
         <v>11</v>
@@ -1055,7 +1056,7 @@
         <v>20</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I9" s="5">
         <v>10</v>
@@ -1083,7 +1084,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5">
         <v>8</v>
@@ -1125,10 +1126,10 @@
         <v>49</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10">
@@ -1153,7 +1154,7 @@
         <v>64</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1165,10 +1166,10 @@
         <v>54</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1191,7 +1192,7 @@
         <v>64</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1203,10 +1204,10 @@
         <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
@@ -1231,7 +1232,7 @@
         <v>64</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1243,17 +1244,17 @@
         <v>49</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
         <v>12</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I14" s="5">
         <v>8</v>
@@ -1269,7 +1270,7 @@
         <v>64</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1281,10 +1282,10 @@
         <v>55</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5">
@@ -1307,7 +1308,7 @@
         <v>64</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1319,10 +1320,10 @@
         <v>56</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16">
@@ -1345,7 +1346,7 @@
         <v>64</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1358,17 +1359,21 @@
       <c r="C17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>77</v>
+      <c r="D17" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E17" s="5">
         <v>9</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="24" t="s">
+        <v>48</v>
+      </c>
       <c r="G17" s="10">
         <v>32</v>
       </c>
-      <c r="H17" s="10"/>
+      <c r="H17" s="24" t="s">
+        <v>48</v>
+      </c>
       <c r="I17" s="10">
         <v>9</v>
       </c>
@@ -1395,16 +1400,20 @@
         <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E18" s="5">
         <v>8</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="G18" s="5">
         <v>30</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="I18" s="5">
         <v>8</v>
       </c>
@@ -1431,14 +1440,18 @@
         <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="I19" s="5">
         <v>9</v>
       </c>
@@ -1465,16 +1478,20 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E20" s="5">
         <v>7</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="G20" s="5">
         <v>32</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="I20" s="5">
         <v>8</v>
       </c>
@@ -1500,15 +1517,19 @@
       <c r="C21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>77</v>
+      <c r="D21" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="E21" s="16">
         <v>8</v>
       </c>
-      <c r="F21" s="16"/>
+      <c r="F21" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="17" t="s">
+        <v>73</v>
+      </c>
       <c r="I21" s="16">
         <v>8</v>
       </c>
@@ -1537,7 +1558,7 @@
         <v>50</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E22" s="10">
         <v>16</v>
@@ -1577,7 +1598,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E23" s="5">
         <v>19</v>
@@ -1615,7 +1636,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E24" s="5">
         <v>21</v>
@@ -1655,7 +1676,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E25" s="5">
         <v>22</v>
@@ -1693,7 +1714,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E26" s="5">
         <v>26</v>
@@ -1703,7 +1724,7 @@
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I26" s="5">
         <v>8</v>
@@ -1731,7 +1752,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E27" s="5">
         <v>16</v>
@@ -1769,7 +1790,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E28" s="5">
         <v>19</v>
@@ -1779,7 +1800,7 @@
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="I28" s="5">
         <v>7</v>
@@ -1806,8 +1827,8 @@
       <c r="C29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>78</v>
+      <c r="D29" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="E29" s="16">
         <v>26</v>
@@ -1847,7 +1868,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>66</v>
@@ -1885,7 +1906,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>70</v>
@@ -1923,7 +1944,7 @@
         <v>52</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E32" s="16" t="s">
         <v>68</v>
@@ -1963,7 +1984,7 @@
         <v>53</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E33" s="10">
         <v>140</v>
@@ -1975,7 +1996,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I33" s="10">
         <v>15</v>
@@ -2003,7 +2024,7 @@
         <v>49</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E34" s="5">
         <v>70</v>
@@ -2013,7 +2034,7 @@
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I34" s="5">
         <v>15</v>
@@ -2041,7 +2062,7 @@
         <v>49</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E35" s="5">
         <v>50</v>
@@ -2079,7 +2100,7 @@
         <v>49</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E36" s="16">
         <v>30</v>
@@ -2121,7 +2142,7 @@
         <v>50</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E37" s="10">
         <v>20</v>
@@ -2161,7 +2182,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E38" s="5">
         <v>28</v>
@@ -2173,7 +2194,7 @@
         <v>100</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I38" s="5">
         <v>8</v>
@@ -2201,7 +2222,7 @@
         <v>50</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E39" s="5">
         <v>21</v>
@@ -2241,19 +2262,19 @@
         <v>50</v>
       </c>
       <c r="D40" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="16">
+        <v>19</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>79</v>
-      </c>
-      <c r="E40" s="16">
-        <v>22</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="G40" s="16">
         <v>100</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I40" s="16">
         <v>8</v>
@@ -2276,6 +2297,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A4:A10"/>
@@ -2284,8 +2307,6 @@
     <mergeCell ref="A22:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A36"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reduced bounciness of grenades.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="98">
   <si>
     <t>M9</t>
   </si>
@@ -281,9 +281,6 @@
     <t>5x4/8x6/2x2</t>
   </si>
   <si>
-    <t>5x8/8x6/2x2</t>
-  </si>
-  <si>
     <t>5x4/8x5/1x2</t>
   </si>
   <si>
@@ -306,6 +303,12 @@
   </si>
   <si>
     <t>Additional damage multiplieris applied for sniper rifles (2x)</t>
+  </si>
+  <si>
+    <t>200/450/600</t>
+  </si>
+  <si>
+    <t>5x8/10x6/2x2</t>
   </si>
 </sst>
 </file>
@@ -417,6 +420,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -428,9 +434,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,42 +757,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
+      <c r="A2" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -834,7 +837,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -844,7 +847,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" s="10">
         <v>8</v>
@@ -876,7 +879,7 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -884,7 +887,7 @@
         <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="5">
         <v>11</v>
@@ -916,7 +919,7 @@
       <c r="N5" s="3"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
@@ -924,7 +927,7 @@
         <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E6" s="5">
         <v>17</v>
@@ -956,7 +959,7 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
@@ -964,7 +967,7 @@
         <v>49</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E7" s="5">
         <v>26</v>
@@ -996,7 +999,7 @@
       <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E8" s="5">
         <v>11</v>
@@ -1036,7 +1039,7 @@
       <c r="N8" s="3"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>50</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E9" s="5">
         <v>11</v>
@@ -1076,7 +1079,7 @@
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E10" s="5">
         <v>8</v>
@@ -1116,7 +1119,7 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1126,7 +1129,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>86</v>
@@ -1158,7 +1161,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>54</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>86</v>
@@ -1196,7 +1199,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
@@ -1204,7 +1207,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>87</v>
@@ -1236,7 +1239,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
@@ -1244,10 +1247,10 @@
         <v>49</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5">
@@ -1274,7 +1277,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
@@ -1282,10 +1285,10 @@
         <v>55</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5">
@@ -1312,7 +1315,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
@@ -1320,10 +1323,10 @@
         <v>56</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16">
@@ -1346,11 +1349,11 @@
         <v>64</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1360,7 +1363,7 @@
         <v>50</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" s="5">
         <v>9</v>
@@ -1392,7 +1395,7 @@
       <c r="N17" s="2"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="12" t="s">
         <v>16</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E18" s="5">
         <v>8</v>
@@ -1432,7 +1435,7 @@
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="12" t="s">
         <v>17</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>50</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E19" s="5">
         <v>8</v>
@@ -1470,7 +1473,7 @@
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="12" t="s">
         <v>18</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" s="5">
         <v>7</v>
@@ -1510,7 +1513,7 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="33"/>
       <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
@@ -1518,7 +1521,7 @@
         <v>50</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="16">
         <v>8</v>
@@ -1548,7 +1551,7 @@
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="31" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="9" t="s">
@@ -1558,7 +1561,7 @@
         <v>50</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="10">
         <v>16</v>
@@ -1590,7 +1593,7 @@
       <c r="N22" s="2"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>51</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="5">
         <v>19</v>
@@ -1628,7 +1631,7 @@
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E24" s="5">
         <v>21</v>
@@ -1668,7 +1671,7 @@
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>50</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E25" s="5">
         <v>22</v>
@@ -1706,7 +1709,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
@@ -1714,7 +1717,7 @@
         <v>50</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E26" s="5">
         <v>26</v>
@@ -1744,7 +1747,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="12" t="s">
         <v>21</v>
       </c>
@@ -1752,7 +1755,7 @@
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E27" s="5">
         <v>16</v>
@@ -1782,7 +1785,7 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="12" t="s">
         <v>27</v>
       </c>
@@ -1790,7 +1793,7 @@
         <v>50</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" s="5">
         <v>19</v>
@@ -1820,7 +1823,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="32"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="15" t="s">
         <v>28</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>49</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" s="16">
         <v>26</v>
@@ -1858,7 +1861,7 @@
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="9" t="s">
@@ -1868,7 +1871,7 @@
         <v>52</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>66</v>
@@ -1898,7 +1901,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="12" t="s">
         <v>32</v>
       </c>
@@ -1936,7 +1939,7 @@
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="15" t="s">
         <v>33</v>
       </c>
@@ -1974,7 +1977,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="31" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="9" t="s">
@@ -2016,7 +2019,7 @@
       <c r="N33" s="2"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="12" t="s">
         <v>36</v>
       </c>
@@ -2054,7 +2057,7 @@
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="12" t="s">
         <v>37</v>
       </c>
@@ -2092,7 +2095,7 @@
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="32"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
@@ -2132,7 +2135,7 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="9" t="s">
@@ -2174,7 +2177,7 @@
       <c r="N37" s="2"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
+      <c r="A38" s="32"/>
       <c r="B38" s="12" t="s">
         <v>41</v>
       </c>
@@ -2214,7 +2217,7 @@
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+      <c r="A39" s="32"/>
       <c r="B39" s="12" t="s">
         <v>42</v>
       </c>
@@ -2254,7 +2257,7 @@
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="32"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="15" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Added three more resolutions to the supported resolutions list.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -308,7 +308,7 @@
     <t>200/450/600</t>
   </si>
   <si>
-    <t>5x8/10x6/2x2</t>
+    <t>5x8/11x6/2x2</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Reflected last revision into the balance sheet.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,7 +1990,7 @@
         <v>77</v>
       </c>
       <c r="E33" s="10">
-        <v>140</v>
+        <v>210</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>65</v>
@@ -2030,7 +2030,7 @@
         <v>77</v>
       </c>
       <c r="E34" s="5">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>64</v>
@@ -2068,7 +2068,7 @@
         <v>77</v>
       </c>
       <c r="E35" s="5">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>64</v>
@@ -2106,7 +2106,7 @@
         <v>77</v>
       </c>
       <c r="E36" s="16">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F36" s="16" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Increased Intervention damage by 33%.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="4440" windowHeight="2100"/>
+    <workbookView xWindow="120" yWindow="210" windowWidth="4440" windowHeight="2040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -1990,7 +1990,7 @@
         <v>77</v>
       </c>
       <c r="E33" s="10">
-        <v>210</v>
+        <v>280</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Updated balance table to include rarities.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="210" windowWidth="4440" windowHeight="2040"/>
+    <workbookView xWindow="120" yWindow="270" windowWidth="4440" windowHeight="1980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="103">
   <si>
     <t>M9</t>
   </si>
@@ -302,13 +302,28 @@
     <t>Last updated 16.3. (r268)</t>
   </si>
   <si>
-    <t>Additional damage multiplieris applied for sniper rifles (2x)</t>
-  </si>
-  <si>
     <t>200/450/600</t>
   </si>
   <si>
     <t>5x8/11x6/2x2</t>
+  </si>
+  <si>
+    <t>Rar- ity</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R </t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Rarities: C = Common, U = Uncomon, R = Rare</t>
   </si>
 </sst>
 </file>
@@ -372,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -420,6 +435,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -434,6 +452,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,1573 +757,1698 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="29" t="s">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-    </row>
-    <row r="3" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F4" s="10">
         <v>8</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="10">
+      <c r="G4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="10">
         <v>15</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="10">
         <v>10</v>
       </c>
-      <c r="J4" s="10">
+      <c r="K4" s="10">
         <v>20</v>
       </c>
-      <c r="K4" s="10">
+      <c r="L4" s="10">
         <v>2</v>
       </c>
-      <c r="L4" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="M4" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="5">
+      <c r="F5" s="5">
         <v>11</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="G5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="5">
         <v>12</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="5">
         <v>10</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>20</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>2</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
+      <c r="M5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
       <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="5">
+      <c r="F6" s="5">
         <v>17</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="G6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="5">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>10</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>20</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <v>2</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="M6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
       <c r="B7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>26</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="G7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="5">
         <v>7</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="5">
         <v>15</v>
       </c>
-      <c r="J7" s="5">
+      <c r="K7" s="5">
         <v>30</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <v>3</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="M7" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="Q7" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
       <c r="B8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="5">
+      <c r="F8" s="5">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="G8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="5">
         <v>20</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>10</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>20</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>2</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
+      <c r="M8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
       <c r="B9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="5">
+      <c r="F9" s="5">
         <v>11</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>20</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="5">
         <v>10</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>20</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
         <v>3</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>9</v>
       </c>
-      <c r="M9" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="N9" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
       <c r="B10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="5">
+      <c r="F10" s="5">
         <v>8</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="16">
+      <c r="H10" s="16">
         <v>20</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="I10" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="16">
+      <c r="J10" s="16">
         <v>10</v>
       </c>
-      <c r="J10" s="16">
+      <c r="K10" s="16">
         <v>20</v>
       </c>
-      <c r="K10" s="16">
+      <c r="L10" s="16">
         <v>3</v>
       </c>
-      <c r="L10" s="16">
+      <c r="M10" s="16">
         <v>9</v>
       </c>
-      <c r="M10" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="N10" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10">
         <v>4</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="I11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="10">
+      <c r="J11" s="10">
         <v>6</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="10">
+      <c r="K11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="10">
         <v>5</v>
       </c>
-      <c r="L11" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N11" s="5" t="s">
+      <c r="M11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
       <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="F12" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>6</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K12" s="5">
+      <c r="K12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="5">
         <v>5</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" s="5" t="s">
+      <c r="M12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
       <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="F13" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
         <v>8</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="I13" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>7</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K13" s="5">
+      <c r="K13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L13" s="5">
         <v>5</v>
       </c>
-      <c r="L13" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="5" t="s">
+      <c r="M13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
       <c r="B14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="F14" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
         <v>12</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="5">
+      <c r="J14" s="5">
         <v>8</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N14" s="5" t="s">
+      <c r="K14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
       <c r="B15" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="F15" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5">
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
         <v>2</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="5">
         <v>10</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M15" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N15" s="5" t="s">
+      <c r="K15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
       <c r="B16" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16">
+      <c r="F16" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
         <v>5</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="I16" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="16">
+      <c r="J16" s="16">
         <v>8</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="K16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="5">
+      <c r="F17" s="5">
         <v>9</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="G17" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="10">
+      <c r="H17" s="10">
         <v>32</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="I17" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="10">
+      <c r="J17" s="10">
         <v>9</v>
       </c>
-      <c r="J17" s="21">
+      <c r="K17" s="21">
         <v>40311</v>
       </c>
-      <c r="K17" s="21">
+      <c r="L17" s="21">
         <v>40300</v>
       </c>
-      <c r="L17" s="10">
+      <c r="M17" s="10">
         <v>7</v>
       </c>
-      <c r="M17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N17" s="2"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="N17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="5">
+      <c r="F18" s="5">
         <v>8</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="5">
+      <c r="H18" s="5">
         <v>30</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>8</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>12</v>
       </c>
-      <c r="K18" s="22">
+      <c r="L18" s="22">
         <v>40299</v>
       </c>
-      <c r="L18" s="5">
+      <c r="M18" s="5">
         <v>5</v>
       </c>
-      <c r="M18" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
+      <c r="N18" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
       <c r="B19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="5">
+      <c r="F19" s="5">
         <v>8</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="5">
         <v>9</v>
       </c>
-      <c r="J19" s="22">
+      <c r="K19" s="22">
         <v>40311</v>
       </c>
-      <c r="K19" s="22">
+      <c r="L19" s="22">
         <v>40300</v>
       </c>
-      <c r="L19" s="5">
+      <c r="M19" s="5">
         <v>7</v>
       </c>
-      <c r="M19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
+      <c r="N19" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="5">
+      <c r="F20" s="5">
         <v>7</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="5">
+      <c r="H20" s="5">
         <v>32</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="I20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="5">
         <v>8</v>
       </c>
-      <c r="J20" s="5">
+      <c r="K20" s="5">
         <v>12</v>
       </c>
-      <c r="K20" s="22">
+      <c r="L20" s="22">
         <v>40299</v>
       </c>
-      <c r="L20" s="5">
+      <c r="M20" s="5">
         <v>5</v>
       </c>
-      <c r="M20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="N20" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
       <c r="B21" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="16">
+      <c r="F21" s="16">
         <v>8</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="G21" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I21" s="16">
+      <c r="J21" s="16">
         <v>8</v>
       </c>
-      <c r="J21" s="16">
+      <c r="K21" s="16">
         <v>12</v>
       </c>
-      <c r="K21" s="23">
+      <c r="L21" s="23">
         <v>2</v>
       </c>
-      <c r="L21" s="16">
+      <c r="M21" s="16">
         <v>6</v>
       </c>
-      <c r="M21" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="N21" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O21" s="4"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="10">
+      <c r="F22" s="10">
         <v>16</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="G22" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="10">
+      <c r="H22" s="10">
         <v>20</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="10">
+      <c r="J22" s="10">
         <v>7</v>
       </c>
-      <c r="J22" s="21">
+      <c r="K22" s="21">
         <v>40308</v>
       </c>
-      <c r="K22" s="10">
+      <c r="L22" s="10">
         <v>1</v>
       </c>
-      <c r="L22" s="10">
+      <c r="M22" s="10">
         <v>4</v>
       </c>
-      <c r="M22" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="N22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
       <c r="B23" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="5">
+      <c r="F23" s="5">
         <v>19</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
+      <c r="G23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="5">
         <v>7</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" s="5">
+      <c r="K23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="5">
         <v>0.5</v>
       </c>
-      <c r="L23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="M23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E24" s="5">
+      <c r="F24" s="5">
         <v>21</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="G24" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="5">
+      <c r="H24" s="5">
         <v>20</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I24" s="5">
+      <c r="J24" s="5">
         <v>7</v>
       </c>
-      <c r="J24" s="22">
+      <c r="K24" s="22">
         <v>40308</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>0.5</v>
       </c>
-      <c r="L24" s="5">
+      <c r="M24" s="5">
         <v>3</v>
       </c>
-      <c r="M24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="N24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
       <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E25" s="5">
+      <c r="F25" s="5">
         <v>22</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="G25" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="5"/>
+      <c r="I25" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="I25" s="5">
+      <c r="J25" s="5">
         <v>7</v>
       </c>
-      <c r="J25" s="22">
+      <c r="K25" s="22">
         <v>40308</v>
       </c>
-      <c r="K25" s="5">
+      <c r="L25" s="5">
         <v>1</v>
       </c>
-      <c r="L25" s="5">
+      <c r="M25" s="5">
         <v>4</v>
       </c>
-      <c r="M25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="N25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
       <c r="B26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="5">
+      <c r="F26" s="5">
         <v>26</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="G26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="5"/>
+      <c r="I26" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="5">
+      <c r="J26" s="5">
         <v>8</v>
       </c>
-      <c r="J26" s="5">
+      <c r="K26" s="5">
         <v>12</v>
       </c>
-      <c r="K26" s="5">
+      <c r="L26" s="5">
         <v>1.5</v>
       </c>
-      <c r="L26" s="5">
+      <c r="M26" s="5">
         <v>5</v>
       </c>
-      <c r="M26" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="N26" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
       <c r="B27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="5">
+      <c r="F27" s="5">
         <v>16</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="14" t="s">
+      <c r="G27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I27" s="5">
+      <c r="J27" s="5">
         <v>7</v>
       </c>
-      <c r="J27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K27" s="5">
+      <c r="K27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" s="5">
         <v>1</v>
       </c>
-      <c r="L27" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M27" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="M27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
       <c r="B28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="5">
+      <c r="F28" s="5">
         <v>19</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="G28" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I28" s="5">
+      <c r="J28" s="5">
         <v>7</v>
       </c>
-      <c r="J28" s="22">
+      <c r="K28" s="22">
         <v>40308</v>
       </c>
-      <c r="K28" s="5">
+      <c r="L28" s="5">
         <v>0.5</v>
       </c>
-      <c r="L28" s="5">
+      <c r="M28" s="5">
         <v>3</v>
       </c>
-      <c r="M28" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+      <c r="N28" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
       <c r="B29" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="16">
+      <c r="F29" s="16">
         <v>26</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17" t="s">
+      <c r="G29" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="16">
+      <c r="J29" s="16">
         <v>7</v>
       </c>
-      <c r="J29" s="25">
+      <c r="K29" s="25">
         <v>40308</v>
       </c>
-      <c r="K29" s="16">
+      <c r="L29" s="16">
         <v>0.5</v>
       </c>
-      <c r="L29" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M29" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N29" s="4"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="M29" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O29" s="4"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="E30" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="G30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="10">
+      <c r="H30" s="10">
         <v>1</v>
       </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="I30" s="10"/>
       <c r="J30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N30" s="2" t="s">
+      <c r="K30" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O30" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
       <c r="B31" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="F31" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="G31" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="5">
+      <c r="H31" s="5">
         <v>1</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>64</v>
-      </c>
+      <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M31" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N31" s="3" t="s">
+      <c r="K31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O31" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
       <c r="B32" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="E32" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="F32" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="G32" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G32" s="16">
+      <c r="H32" s="16">
         <v>1</v>
       </c>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="I32" s="16"/>
       <c r="J32" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M32" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N32" s="4" t="s">
+      <c r="K32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N32" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O32" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
         <v>39</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="10">
+      <c r="F33" s="10">
         <v>280</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="G33" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G33" s="10">
+      <c r="H33" s="10">
         <v>5</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="I33" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I33" s="10">
+      <c r="J33" s="10">
         <v>15</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K33" s="10">
+      <c r="K33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="L33" s="10">
         <v>0</v>
       </c>
-      <c r="L33" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M33" s="10">
+      <c r="M33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="10">
         <v>6</v>
       </c>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
       <c r="B34" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="5">
+      <c r="F34" s="5">
         <v>105</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="14" t="s">
+      <c r="G34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="I34" s="5">
+      <c r="J34" s="5">
         <v>15</v>
       </c>
-      <c r="J34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K34" s="5">
+      <c r="K34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L34" s="5">
         <v>0</v>
       </c>
-      <c r="L34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M34" s="5">
+      <c r="M34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="5">
         <v>6</v>
       </c>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="32"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
       <c r="B35" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="5">
+      <c r="F35" s="5">
         <v>75</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="14" t="s">
+      <c r="G35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="5">
+      <c r="J35" s="5">
         <v>15</v>
       </c>
-      <c r="J35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K35" s="5">
+      <c r="K35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L35" s="5">
         <v>0</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M35" s="5">
+      <c r="M35" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="N35" s="5">
         <v>6</v>
       </c>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
       <c r="B36" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="E36" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="16">
+      <c r="F36" s="16">
         <v>45</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="G36" s="16">
+      <c r="G36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="16">
         <v>10</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="I36" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="I36" s="16">
+      <c r="J36" s="16">
         <v>15</v>
       </c>
-      <c r="J36" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K36" s="16">
+      <c r="K36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="L36" s="16">
         <v>0</v>
       </c>
-      <c r="L36" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="M36" s="16">
+      <c r="M36" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N36" s="16">
         <v>6</v>
       </c>
-      <c r="N36" s="4"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="O36" s="4"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="10">
+      <c r="F37" s="10">
         <v>20</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="G37" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="10">
+      <c r="H37" s="10">
         <v>100</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="I37" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I37" s="10">
+      <c r="J37" s="10">
         <v>7</v>
       </c>
-      <c r="J37" s="21">
+      <c r="K37" s="21">
         <v>40308</v>
       </c>
-      <c r="K37" s="10">
+      <c r="L37" s="10">
         <v>1</v>
       </c>
-      <c r="L37" s="21">
+      <c r="M37" s="21">
         <v>40300</v>
       </c>
-      <c r="M37" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="N37" s="2"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="32"/>
+      <c r="N37" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
       <c r="B38" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="5">
+      <c r="F38" s="5">
         <v>28</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="G38" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G38" s="5">
+      <c r="H38" s="5">
         <v>100</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="I38" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I38" s="5">
+      <c r="J38" s="5">
         <v>8</v>
       </c>
-      <c r="J38" s="26">
+      <c r="K38" s="26">
         <v>12</v>
       </c>
-      <c r="K38" s="5">
+      <c r="L38" s="5">
         <v>2</v>
       </c>
-      <c r="L38" s="22">
+      <c r="M38" s="22">
         <v>40301</v>
       </c>
-      <c r="M38" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="32"/>
+      <c r="N38" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
       <c r="B39" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="5">
+      <c r="F39" s="5">
         <v>21</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="G39" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G39" s="5">
+      <c r="H39" s="5">
         <v>100</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="I39" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="I39" s="5">
+      <c r="J39" s="5">
         <v>7</v>
       </c>
-      <c r="J39" s="22">
+      <c r="K39" s="22">
         <v>40308</v>
       </c>
-      <c r="K39" s="5">
+      <c r="L39" s="5">
         <v>1</v>
       </c>
-      <c r="L39" s="22">
+      <c r="M39" s="22">
         <v>40300</v>
       </c>
-      <c r="M39" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="N39" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
       <c r="B40" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="E40" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="16">
+      <c r="F40" s="16">
         <v>19</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="G40" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="G40" s="16">
+      <c r="H40" s="16">
         <v>100</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="I40" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="I40" s="16">
+      <c r="J40" s="16">
         <v>8</v>
       </c>
-      <c r="J40" s="16">
+      <c r="K40" s="16">
         <v>12</v>
       </c>
-      <c r="K40" s="16">
+      <c r="L40" s="16">
         <v>2</v>
       </c>
-      <c r="L40" s="25">
+      <c r="M40" s="25">
         <v>40301</v>
       </c>
-      <c r="M40" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="N40" s="4" t="s">
+      <c r="N40" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="O40" s="4" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:N2"/>
+  <mergeCells count="11">
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="Q7:AE7"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="A11:A16"/>
@@ -2310,6 +2456,8 @@
     <mergeCell ref="A22:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed weapon balance sheet date.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -299,9 +299,6 @@
     <t>100/70%</t>
   </si>
   <si>
-    <t>Last updated 16.3. (r268)</t>
-  </si>
-  <si>
     <t>200/450/600</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Rarities: C = Common, U = Uncomon, R = Rare</t>
+  </si>
+  <si>
+    <t>Last updated 4.6. (r476)</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A10"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +780,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -793,7 +793,7 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="30" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -816,7 +816,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>45</v>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>49</v>
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
@@ -949,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -992,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
@@ -1052,7 +1052,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>51</v>
@@ -1095,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>50</v>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>50</v>
@@ -1183,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>49</v>
@@ -1226,7 +1226,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>54</v>
@@ -1267,7 +1267,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
@@ -1351,7 +1351,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>55</v>
@@ -1392,7 +1392,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>56</v>
@@ -1401,7 +1401,7 @@
         <v>92</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16">
@@ -1424,7 +1424,7 @@
         <v>64</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>50</v>
@@ -1478,7 +1478,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>50</v>
@@ -1521,7 +1521,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>50</v>
@@ -1562,7 +1562,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>50</v>
@@ -1605,7 +1605,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>50</v>
@@ -1648,7 +1648,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>50</v>
@@ -1691,7 +1691,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>51</v>
@@ -1732,7 +1732,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>50</v>
@@ -1775,7 +1775,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>50</v>
@@ -1816,7 +1816,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>50</v>
@@ -1857,7 +1857,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>51</v>
@@ -1898,7 +1898,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>50</v>
@@ -1939,7 +1939,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>49</v>
@@ -1982,7 +1982,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>52</v>
@@ -2023,7 +2023,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>52</v>
@@ -2064,7 +2064,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>52</v>
@@ -2107,7 +2107,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>53</v>
@@ -2150,7 +2150,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
@@ -2191,7 +2191,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>49</v>
@@ -2232,7 +2232,7 @@
         <v>38</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>49</v>
@@ -2277,7 +2277,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>50</v>
@@ -2320,7 +2320,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>50</v>
@@ -2363,7 +2363,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>50</v>
@@ -2406,7 +2406,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Fixed clip vs. magazine in the balance table.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -323,7 +323,7 @@
     <t>Rarities: C = Common, U = Uncomon, R = Rare</t>
   </si>
   <si>
-    <t>Last updated 4.6. (r476)</t>
+    <t>Last updated 13.6. (r476)</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1153,7 @@
         <v>73</v>
       </c>
       <c r="H10" s="16">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
M14 EBR is now fully automatic.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -323,7 +323,7 @@
     <t>Rarities: C = Common, U = Uncomon, R = Rare</t>
   </si>
   <si>
-    <t>Last updated 13.6. (r476)</t>
+    <t>Last updated 16.6. (r504)</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="L1" sqref="L1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2164,7 +2164,9 @@
       <c r="G34" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5">
+        <v>10</v>
+      </c>
       <c r="I34" s="14" t="s">
         <v>80</v>
       </c>
@@ -2205,7 +2207,9 @@
       <c r="G35" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H35" s="5"/>
+      <c r="H35" s="5">
+        <v>5</v>
+      </c>
       <c r="I35" s="14" t="s">
         <v>73</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>99</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E36" s="16" t="s">
         <v>77</v>
@@ -2247,7 +2251,7 @@
         <v>64</v>
       </c>
       <c r="H36" s="16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Increased M14 damage by 9%.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:O1"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2245,7 +2245,7 @@
         <v>77</v>
       </c>
       <c r="F36" s="16">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G36" s="16" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Increased M14 movement speed by 25%.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="104">
   <si>
     <t>M9</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Last updated 16.6. (r504)</t>
+  </si>
+  <si>
+    <t>80/30%</t>
   </si>
 </sst>
 </file>
@@ -760,7 +763,7 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,7 +2245,7 @@
         <v>50</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="F36" s="16">
         <v>50</v>

</xml_diff>

<commit_message>
Added recent change to AA12 to the balance table.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -278,9 +279,6 @@
     <t>5x5/8x7/2x2</t>
   </si>
   <si>
-    <t>5x4/8x6/2x2</t>
-  </si>
-  <si>
     <t>5x4/8x5/1x2</t>
   </si>
   <si>
@@ -327,6 +325,9 @@
   </si>
   <si>
     <t>80/30%</t>
+  </si>
+  <si>
+    <t>5x4/7x6/2x2</t>
   </si>
 </sst>
 </file>
@@ -762,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +784,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -796,7 +797,7 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -804,7 +805,7 @@
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -819,7 +820,7 @@
         <v>57</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>45</v>
@@ -866,13 +867,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="10">
         <v>8</v>
@@ -909,13 +910,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="5">
         <v>11</v>
@@ -952,13 +953,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="5">
         <v>17</v>
@@ -995,13 +996,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="5">
         <v>26</v>
@@ -1055,13 +1056,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="5">
         <v>11</v>
@@ -1098,13 +1099,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="5">
         <v>11</v>
@@ -1141,13 +1142,13 @@
         <v>6</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F10" s="5">
         <v>8</v>
@@ -1186,13 +1187,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="19" t="s">
         <v>86</v>
@@ -1229,13 +1230,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>86</v>
@@ -1270,16 +1271,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
@@ -1313,16 +1314,16 @@
         <v>11</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
@@ -1354,16 +1355,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
@@ -1395,16 +1396,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16">
@@ -1427,7 +1428,7 @@
         <v>64</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1438,13 +1439,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" s="5">
         <v>9</v>
@@ -1481,13 +1482,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="5">
         <v>8</v>
@@ -1524,13 +1525,13 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F19" s="5">
         <v>8</v>
@@ -1565,13 +1566,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="5">
         <v>7</v>
@@ -1608,13 +1609,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" s="16">
         <v>8</v>
@@ -1651,13 +1652,13 @@
         <v>22</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F22" s="10">
         <v>16</v>
@@ -1694,13 +1695,13 @@
         <v>23</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F23" s="5">
         <v>19</v>
@@ -1735,13 +1736,13 @@
         <v>24</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F24" s="5">
         <v>21</v>
@@ -1778,13 +1779,13 @@
         <v>25</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F25" s="5">
         <v>22</v>
@@ -1819,13 +1820,13 @@
         <v>26</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F26" s="5">
         <v>26</v>
@@ -1860,13 +1861,13 @@
         <v>21</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F27" s="5">
         <v>16</v>
@@ -1901,13 +1902,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F28" s="5">
         <v>19</v>
@@ -1942,13 +1943,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F29" s="16">
         <v>26</v>
@@ -1985,13 +1986,13 @@
         <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>52</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>66</v>
@@ -2026,7 +2027,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>52</v>
@@ -2067,7 +2068,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>52</v>
@@ -2110,7 +2111,7 @@
         <v>35</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>53</v>
@@ -2153,7 +2154,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
@@ -2196,7 +2197,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>49</v>
@@ -2239,13 +2240,13 @@
         <v>38</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F36" s="16">
         <v>50</v>
@@ -2284,7 +2285,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>50</v>
@@ -2327,7 +2328,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>50</v>
@@ -2370,7 +2371,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>50</v>
@@ -2413,7 +2414,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Increased Thumper damage by 90%, slightly decreased blast radius.
</commit_message>
<xml_diff>
--- a/weapon balance sheet.xlsx
+++ b/weapon balance sheet.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -216,12 +215,6 @@
     <t>---</t>
   </si>
   <si>
-    <t>150 + 150</t>
-  </si>
-  <si>
-    <t>170 + 300</t>
-  </si>
-  <si>
     <t>500 + 250 + 100</t>
   </si>
   <si>
@@ -321,13 +314,19 @@
     <t>Rarities: C = Common, U = Uncomon, R = Rare</t>
   </si>
   <si>
-    <t>Last updated 16.6. (r504)</t>
-  </si>
-  <si>
     <t>80/30%</t>
   </si>
   <si>
     <t>5x4/7x6/2x2</t>
+  </si>
+  <si>
+    <t>340 + 150</t>
+  </si>
+  <si>
+    <t>40 + 100</t>
+  </si>
+  <si>
+    <t>Last updated 30.1. (r627)</t>
   </si>
 </sst>
 </file>
@@ -764,7 +763,7 @@
   <dimension ref="A1:AE40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +783,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -797,7 +796,7 @@
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>
       <c r="L1" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
@@ -805,7 +804,7 @@
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -820,13 +819,13 @@
         <v>57</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>46</v>
@@ -838,7 +837,7 @@
         <v>58</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>59</v>
@@ -850,13 +849,13 @@
         <v>61</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>62</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -867,13 +866,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F4" s="10">
         <v>8</v>
@@ -910,13 +909,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" s="5">
         <v>11</v>
@@ -953,13 +952,13 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="5">
         <v>17</v>
@@ -971,7 +970,7 @@
         <v>6</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J6" s="5">
         <v>10</v>
@@ -996,13 +995,13 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5">
         <v>26</v>
@@ -1014,7 +1013,7 @@
         <v>7</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7" s="5">
         <v>15</v>
@@ -1056,13 +1055,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="5">
         <v>11</v>
@@ -1099,25 +1098,25 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F9" s="5">
         <v>11</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H9" s="5">
         <v>20</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J9" s="5">
         <v>10</v>
@@ -1142,25 +1141,25 @@
         <v>6</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" s="5">
         <v>8</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H10" s="16">
         <v>33</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J10" s="16">
         <v>10</v>
@@ -1187,23 +1186,23 @@
         <v>8</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10">
         <v>4</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J11" s="10">
         <v>6</v>
@@ -1221,7 +1220,7 @@
         <v>64</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -1230,21 +1229,21 @@
         <v>9</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J12" s="5">
         <v>6</v>
@@ -1262,7 +1261,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -1271,23 +1270,23 @@
         <v>10</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5">
         <v>8</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J13" s="5">
         <v>7</v>
@@ -1305,7 +1304,7 @@
         <v>64</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -1314,23 +1313,23 @@
         <v>11</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5">
         <v>12</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J14" s="5">
         <v>8</v>
@@ -1346,7 +1345,7 @@
         <v>64</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -1355,23 +1354,23 @@
         <v>12</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5">
         <v>2</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J15" s="5">
         <v>10</v>
@@ -1387,7 +1386,7 @@
         <v>64</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -1396,23 +1395,23 @@
         <v>13</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16">
         <v>5</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J16" s="16">
         <v>8</v>
@@ -1428,7 +1427,7 @@
         <v>64</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1439,13 +1438,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F17" s="5">
         <v>9</v>
@@ -1482,13 +1481,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F18" s="5">
         <v>8</v>
@@ -1525,23 +1524,23 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F19" s="5">
         <v>8</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J19" s="5">
         <v>9</v>
@@ -1566,25 +1565,25 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F20" s="5">
         <v>7</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H20" s="5">
         <v>32</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J20" s="5">
         <v>8</v>
@@ -1609,13 +1608,13 @@
         <v>19</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F21" s="16">
         <v>8</v>
@@ -1625,7 +1624,7 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J21" s="16">
         <v>8</v>
@@ -1652,19 +1651,19 @@
         <v>22</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F22" s="10">
         <v>16</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" s="10">
         <v>20</v>
@@ -1695,13 +1694,13 @@
         <v>23</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F23" s="5">
         <v>19</v>
@@ -1711,7 +1710,7 @@
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J23" s="5">
         <v>7</v>
@@ -1736,13 +1735,13 @@
         <v>24</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F24" s="5">
         <v>21</v>
@@ -1779,23 +1778,23 @@
         <v>25</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F25" s="5">
         <v>22</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J25" s="5">
         <v>7</v>
@@ -1820,23 +1819,23 @@
         <v>26</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F26" s="5">
         <v>26</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J26" s="5">
         <v>8</v>
@@ -1861,13 +1860,13 @@
         <v>21</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="5">
         <v>16</v>
@@ -1902,13 +1901,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F28" s="5">
         <v>19</v>
@@ -1918,7 +1917,7 @@
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J28" s="5">
         <v>7</v>
@@ -1943,13 +1942,13 @@
         <v>28</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F29" s="16">
         <v>26</v>
@@ -1986,16 +1985,16 @@
         <v>30</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>52</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>63</v>
@@ -2018,7 +2017,7 @@
         <v>64</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2027,16 +2026,16 @@
         <v>32</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>52</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G31" s="14" t="s">
         <v>48</v>
@@ -2059,7 +2058,7 @@
         <v>64</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2068,16 +2067,16 @@
         <v>33</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>52</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>65</v>
@@ -2100,7 +2099,7 @@
         <v>64</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2111,13 +2110,13 @@
         <v>35</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F33" s="10">
         <v>280</v>
@@ -2129,7 +2128,7 @@
         <v>5</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J33" s="10">
         <v>15</v>
@@ -2154,13 +2153,13 @@
         <v>36</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F34" s="5">
         <v>105</v>
@@ -2172,7 +2171,7 @@
         <v>10</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J34" s="5">
         <v>15</v>
@@ -2197,13 +2196,13 @@
         <v>37</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F35" s="5">
         <v>75</v>
@@ -2215,7 +2214,7 @@
         <v>5</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J35" s="5">
         <v>15</v>
@@ -2240,13 +2239,13 @@
         <v>38</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F36" s="16">
         <v>50</v>
@@ -2285,13 +2284,13 @@
         <v>40</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F37" s="10">
         <v>20</v>
@@ -2303,7 +2302,7 @@
         <v>100</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J37" s="10">
         <v>7</v>
@@ -2328,13 +2327,13 @@
         <v>41</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F38" s="5">
         <v>28</v>
@@ -2346,7 +2345,7 @@
         <v>100</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J38" s="5">
         <v>8</v>
@@ -2371,25 +2370,25 @@
         <v>42</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F39" s="5">
         <v>21</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H39" s="5">
         <v>100</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J39" s="5">
         <v>7</v>
@@ -2414,25 +2413,25 @@
         <v>43</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F40" s="16">
         <v>19</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H40" s="16">
         <v>100</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J40" s="16">
         <v>8</v>

</xml_diff>